<commit_message>
Add granting to casbin roles
</commit_message>
<xml_diff>
--- a/policy_generator/Roles.xlsx
+++ b/policy_generator/Roles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahdi\Git\GitHub\mra-authorization\casbin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahdi\Git\GitHub\mra-authorization\policy_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8080D9-1D59-4EC2-8157-8E2116662B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D1B9BE-0714-475D-AA26-1F67B07A6DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{252918B9-00B2-423B-B89C-CAD0DFB0D9ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="153">
   <si>
     <t>mra_countries</t>
   </si>
@@ -500,6 +500,24 @@
   </si>
   <si>
     <t>CUD</t>
+  </si>
+  <si>
+    <t>casbin_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A casbin table for managing roles and only modifiable via authorization service. </t>
+  </si>
+  <si>
+    <t>GR*</t>
+  </si>
+  <si>
+    <t>GC*GR*</t>
+  </si>
+  <si>
+    <t>GC*GR*GU*GD*</t>
+  </si>
+  <si>
+    <t>GC*RGU*GD*</t>
   </si>
 </sst>
 </file>
@@ -568,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1179,11 +1197,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1334,6 +1400,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1352,15 +1427,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1678,10 +1759,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V58"/>
+  <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,8 +1782,8 @@
     <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" customWidth="1"/>
     <col min="18" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" customWidth="1"/>
     <col min="21" max="21" width="11.85546875" customWidth="1"/>
@@ -1713,12 +1794,12 @@
       <c r="A1" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="84"/>
       <c r="F1" s="75" t="s">
         <v>137</v>
       </c>
@@ -1727,12 +1808,12 @@
       <c r="A2" s="76">
         <v>1</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
       <c r="F2" s="77" t="s">
         <v>54</v>
       </c>
@@ -1741,12 +1822,12 @@
       <c r="A3" s="67">
         <v>2</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="85" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="83"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="86"/>
       <c r="F3" s="8" t="s">
         <v>47</v>
       </c>
@@ -1755,12 +1836,12 @@
       <c r="A4" s="67">
         <v>3</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="83"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
       <c r="F4" s="8" t="s">
         <v>118</v>
       </c>
@@ -1769,12 +1850,12 @@
       <c r="A5" s="67">
         <v>4</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="83"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
       <c r="F5" s="8" t="s">
         <v>141</v>
       </c>
@@ -1783,12 +1864,12 @@
       <c r="A6" s="67">
         <v>5</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="83"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
       <c r="F6" s="8" t="s">
         <v>146</v>
       </c>
@@ -1797,12 +1878,12 @@
       <c r="A7" s="67">
         <v>6</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="83"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
       <c r="F7" s="31" t="s">
         <v>139</v>
       </c>
@@ -1811,12 +1892,12 @@
       <c r="A8" s="68">
         <v>7</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="87" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="85"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="10" t="s">
         <v>140</v>
       </c>
@@ -1830,42 +1911,48 @@
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="71"/>
-      <c r="H10" s="88" t="s">
+      <c r="H10" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="89"/>
-      <c r="Q10" s="89"/>
-      <c r="R10" s="89"/>
-      <c r="S10" s="89"/>
-      <c r="T10" s="89"/>
-      <c r="U10" s="90"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="83"/>
+      <c r="Q10" s="83"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="83"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="84"/>
       <c r="V10" s="72"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="73"/>
-      <c r="H11" s="88" t="s">
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="89"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="89"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="88" t="s">
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="84"/>
+      <c r="P11" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="89"/>
-      <c r="S11" s="90"/>
+      <c r="Q11" s="83"/>
+      <c r="R11" s="83"/>
+      <c r="S11" s="84"/>
       <c r="T11" s="14" t="s">
         <v>57</v>
       </c>
@@ -1876,6 +1963,12 @@
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="73"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
       <c r="H12" s="17">
         <v>1100</v>
       </c>
@@ -3443,10 +3536,10 @@
         <v>143</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="R36" s="2" t="s">
         <v>118</v>
@@ -3701,10 +3794,10 @@
         <v>139</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R40" s="2" t="s">
         <v>118</v>
@@ -3765,7 +3858,7 @@
         <v>47</v>
       </c>
       <c r="P41" s="21" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>54</v>
@@ -3829,7 +3922,7 @@
         <v>47</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="Q42" s="2" t="s">
         <v>54</v>
@@ -3957,10 +4050,10 @@
         <v>139</v>
       </c>
       <c r="P44" s="21" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="R44" s="2" t="s">
         <v>118</v>
@@ -4021,10 +4114,10 @@
         <v>47</v>
       </c>
       <c r="P45" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R45" s="2" t="s">
         <v>54</v>
@@ -4085,10 +4178,10 @@
         <v>47</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R46" s="2" t="s">
         <v>118</v>
@@ -4149,10 +4242,10 @@
         <v>47</v>
       </c>
       <c r="P47" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R47" s="2" t="s">
         <v>118</v>
@@ -4213,10 +4306,10 @@
         <v>47</v>
       </c>
       <c r="P48" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R48" s="2" t="s">
         <v>118</v>
@@ -4277,10 +4370,10 @@
         <v>139</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R49" s="2" t="s">
         <v>118</v>
@@ -4341,10 +4434,10 @@
         <v>139</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R50" s="2" t="s">
         <v>118</v>
@@ -4405,16 +4498,16 @@
         <v>47</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="T51" s="13" t="s">
         <v>141</v>
@@ -4469,10 +4562,10 @@
         <v>47</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R52" s="2" t="s">
         <v>142</v>
@@ -4533,10 +4626,10 @@
         <v>47</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="R53" s="2" t="s">
         <v>142</v>
@@ -4612,7 +4705,7 @@
         <v>141</v>
       </c>
       <c r="U54" s="23" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="V54" s="33" t="s">
         <v>102</v>
@@ -4789,10 +4882,10 @@
         <v>47</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="R57" s="2" t="s">
         <v>54</v>
@@ -4810,83 +4903,171 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="80">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A58" s="79">
         <v>45</v>
       </c>
-      <c r="B58" s="66" t="s">
+      <c r="B58" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="81" t="s">
+      <c r="C58" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="7">
         <v>0</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="7">
         <v>60</v>
       </c>
-      <c r="F58" s="9"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L58" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M58" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N58" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="O58" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="P58" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q58" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="R58" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="S58" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="T58" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="U58" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="V58" s="35" t="s">
+      <c r="F58" s="7"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P58" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T58" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="U58" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="V58" s="33" t="s">
         <v>110</v>
       </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A59" s="93">
+        <v>46</v>
+      </c>
+      <c r="B59" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" s="94" t="s">
+        <v>128</v>
+      </c>
+      <c r="D59" s="30">
+        <v>700</v>
+      </c>
+      <c r="E59" s="30">
+        <v>800</v>
+      </c>
+      <c r="F59" s="30"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L59" s="96" t="s">
+        <v>47</v>
+      </c>
+      <c r="M59" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="N59" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="O59" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="P59" s="98" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q59" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="R59" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="S59" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="T59" s="99" t="s">
+        <v>54</v>
+      </c>
+      <c r="U59" s="95" t="s">
+        <v>54</v>
+      </c>
+      <c r="V59" s="34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="80"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="81"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="22"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="5"/>
+      <c r="T60" s="6"/>
+      <c r="U60" s="24"/>
+      <c r="V60" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="H11:O11"/>
     <mergeCell ref="P11:S11"/>
     <mergeCell ref="H10:U10"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="35" orientation="landscape" r:id="rId1"/>

</xml_diff>